<commit_message>
Layout + Routing v1 done
</commit_message>
<xml_diff>
--- a/hardware/parts/Parts.xlsx
+++ b/hardware/parts/Parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mois\Documents\GitHub\Mercury\hardware\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1CB841-F676-4055-AB0E-8E69986D17CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2B1C6E-A96A-49EE-9157-A857A2FF5400}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2580" windowWidth="17280" windowHeight="8964" xr2:uid="{15D68DC7-770F-4EC0-8DFC-7BA9B78F8580}"/>
+    <workbookView xWindow="11520" yWindow="96" windowWidth="11448" windowHeight="11448" xr2:uid="{15D68DC7-770F-4EC0-8DFC-7BA9B78F8580}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="275">
   <si>
     <t>Reference Designator</t>
   </si>
@@ -227,9 +227,6 @@
     <t>Estimate</t>
   </si>
   <si>
-    <t>C24</t>
-  </si>
-  <si>
     <t>C25</t>
   </si>
   <si>
@@ -626,12 +623,6 @@
     <t>R23</t>
   </si>
   <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>R25</t>
-  </si>
-  <si>
     <t>R26</t>
   </si>
   <si>
@@ -861,6 +852,12 @@
   </si>
   <si>
     <t>RF HSE</t>
+  </si>
+  <si>
+    <t>C87898</t>
+  </si>
+  <si>
+    <t>LPS25HBTR</t>
   </si>
 </sst>
 </file>
@@ -1248,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D181B8E6-3771-4A93-B031-60F244DC73DC}">
-  <dimension ref="A1:H119"/>
+  <dimension ref="A1:H116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1318,7 +1315,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" t="s">
@@ -1339,7 +1336,7 @@
         <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" t="s">
@@ -1360,7 +1357,7 @@
         <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" t="s">
@@ -1381,7 +1378,7 @@
         <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" t="s">
@@ -1402,7 +1399,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" t="s">
@@ -1423,7 +1420,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" t="s">
@@ -1444,7 +1441,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" t="s">
@@ -1665,7 +1662,7 @@
         <v>23</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" t="s">
@@ -1686,7 +1683,7 @@
         <v>23</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" t="s">
@@ -1707,7 +1704,7 @@
         <v>23</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" t="s">
@@ -1748,7 +1745,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F24" t="s">
         <v>62</v>
@@ -1762,19 +1759,19 @@
         <v>64</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F25" t="s">
         <v>62</v>
       </c>
       <c r="G25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1782,19 +1779,19 @@
         <v>65</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F26" t="s">
         <v>62</v>
       </c>
       <c r="G26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1808,13 +1805,13 @@
         <v>23</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F27" t="s">
         <v>62</v>
       </c>
       <c r="G27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1828,13 +1825,13 @@
         <v>23</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F28" t="s">
         <v>62</v>
       </c>
       <c r="G28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1848,13 +1845,13 @@
         <v>23</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F29" t="s">
         <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1862,19 +1859,19 @@
         <v>69</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F30" t="s">
         <v>62</v>
       </c>
       <c r="G30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1882,19 +1879,19 @@
         <v>70</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="F31" t="s">
         <v>62</v>
       </c>
       <c r="G31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1902,19 +1899,19 @@
         <v>71</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="F32" t="s">
         <v>62</v>
       </c>
       <c r="G32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1922,19 +1919,19 @@
         <v>72</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F33" t="s">
         <v>62</v>
       </c>
       <c r="G33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -1942,19 +1939,19 @@
         <v>73</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="F34" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="G34" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -1974,7 +1971,7 @@
         <v>40</v>
       </c>
       <c r="G35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -1982,19 +1979,19 @@
         <v>75</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="F36" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="G36" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2002,19 +1999,19 @@
         <v>76</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>93</v>
+        <v>38</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="F37" t="s">
         <v>62</v>
       </c>
       <c r="G37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2022,19 +2019,19 @@
         <v>77</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="F38" t="s">
         <v>62</v>
       </c>
       <c r="G38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2042,19 +2039,19 @@
         <v>78</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="F39" t="s">
         <v>62</v>
       </c>
       <c r="G39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2062,19 +2059,19 @@
         <v>79</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>93</v>
+        <v>38</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="F40" t="s">
         <v>62</v>
       </c>
       <c r="G40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2082,19 +2079,19 @@
         <v>80</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="F41" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="G41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2102,19 +2099,19 @@
         <v>81</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2122,19 +2119,19 @@
         <v>82</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D43" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F43" t="s">
         <v>99</v>
       </c>
-      <c r="F43" t="s">
-        <v>101</v>
-      </c>
       <c r="G43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -2142,24 +2139,24 @@
         <v>83</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="F44" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="G44" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>22</v>
@@ -2174,27 +2171,27 @@
         <v>62</v>
       </c>
       <c r="G45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F46" t="s">
+        <v>109</v>
+      </c>
+      <c r="G46" t="s">
         <v>104</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F46" t="s">
-        <v>62</v>
-      </c>
-      <c r="G46" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -2202,99 +2199,99 @@
         <v>106</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D47" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F47" t="s">
         <v>109</v>
       </c>
-      <c r="F47" t="s">
-        <v>110</v>
-      </c>
       <c r="G47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F48" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="G48" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F49" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F50" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="G50" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>31</v>
+        <v>139</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="F51" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="G51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -2302,19 +2299,19 @@
         <v>125</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>138</v>
+      <c r="D52" t="s">
+        <v>116</v>
       </c>
       <c r="F52" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="G52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -2322,19 +2319,19 @@
         <v>126</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D53" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F53" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G53" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -2342,19 +2339,19 @@
         <v>127</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -2362,19 +2359,19 @@
         <v>128</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -2382,19 +2379,19 @@
         <v>129</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -2402,19 +2399,19 @@
         <v>130</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57" t="s">
-        <v>117</v>
+        <v>139</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="F57" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G57" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -2422,19 +2419,19 @@
         <v>131</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="F58" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="G58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -2442,19 +2439,19 @@
         <v>132</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F59" t="s">
         <v>143</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F59" t="s">
-        <v>144</v>
-      </c>
       <c r="G59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -2462,19 +2459,19 @@
         <v>133</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F60" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -2482,19 +2479,19 @@
         <v>134</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F61" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G61" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -2502,239 +2499,239 @@
         <v>135</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F62" t="s">
         <v>143</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F62" t="s">
-        <v>144</v>
-      </c>
       <c r="G62" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>140</v>
+        <v>23</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="F63" t="s">
-        <v>144</v>
+        <v>25</v>
       </c>
       <c r="G63" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F64" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="G64" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>150</v>
+        <v>92</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F65" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F66" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G66" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F67" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G67" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F68" t="s">
-        <v>110</v>
+        <v>162</v>
       </c>
       <c r="G68" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>140</v>
+        <v>23</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F69" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="G69" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>164</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
+      </c>
+      <c r="B70" s="2">
+        <v>47</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F70" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G70" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>168</v>
-      </c>
-      <c r="B71" s="2">
-        <v>47</v>
+        <v>170</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F71" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G71" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D72" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F72" t="s">
         <v>173</v>
       </c>
-      <c r="F72" t="s">
-        <v>174</v>
-      </c>
       <c r="G72" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>177</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="C73" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F73" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G73" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -2742,19 +2739,19 @@
         <v>178</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F74" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -2762,19 +2759,19 @@
         <v>179</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F75" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G75" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -2782,19 +2779,19 @@
         <v>180</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F76" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G76" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -2802,19 +2799,19 @@
         <v>181</v>
       </c>
       <c r="B77" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F77" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G77" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -2822,19 +2819,19 @@
         <v>182</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F78" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G78" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -2842,19 +2839,19 @@
         <v>183</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F79" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G79" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -2862,19 +2859,19 @@
         <v>184</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F80" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G80" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -2882,19 +2879,19 @@
         <v>185</v>
       </c>
       <c r="B81" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F81" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G81" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -2902,19 +2899,19 @@
         <v>186</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F82" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G82" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -2922,19 +2919,19 @@
         <v>187</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F83" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G83" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -2942,19 +2939,19 @@
         <v>188</v>
       </c>
       <c r="B84" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F84" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G84" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -2962,19 +2959,19 @@
         <v>189</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C85" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F85" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G85" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -2982,19 +2979,19 @@
         <v>190</v>
       </c>
       <c r="B86" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F86" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G86" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -3002,19 +2999,19 @@
         <v>191</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F87" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G87" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -3022,19 +3019,19 @@
         <v>192</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F88" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G88" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -3042,19 +3039,19 @@
         <v>193</v>
       </c>
       <c r="B89" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F89" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G89" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -3062,19 +3059,19 @@
         <v>194</v>
       </c>
       <c r="B90" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F90" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G90" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -3082,19 +3079,19 @@
         <v>195</v>
       </c>
       <c r="B91" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C91" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="F91" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G91" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -3102,19 +3099,19 @@
         <v>196</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="F92" t="s">
-        <v>174</v>
+        <v>206</v>
       </c>
       <c r="G92" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -3122,19 +3119,19 @@
         <v>197</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="F93" t="s">
-        <v>174</v>
+        <v>206</v>
       </c>
       <c r="G93" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -3142,19 +3139,19 @@
         <v>198</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="F94" t="s">
-        <v>174</v>
+        <v>206</v>
       </c>
       <c r="G94" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -3162,19 +3159,19 @@
         <v>199</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F95" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G95" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -3182,467 +3179,407 @@
         <v>200</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>208</v>
+        <v>172</v>
       </c>
       <c r="F96" t="s">
-        <v>209</v>
+        <v>173</v>
       </c>
       <c r="G96" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>201</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F97" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G97" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>202</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F98" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G98" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>203</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>172</v>
+        <v>204</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>173</v>
+        <v>205</v>
       </c>
       <c r="F99" t="s">
-        <v>174</v>
+        <v>206</v>
       </c>
       <c r="G99" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D100" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F100" t="s">
+        <v>213</v>
+      </c>
+      <c r="G100" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>208</v>
       </c>
-      <c r="F100" t="s">
+      <c r="B101" s="2">
+        <v>47</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F101" t="s">
+        <v>169</v>
+      </c>
+      <c r="G101" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>209</v>
       </c>
-      <c r="G100" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>205</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F101" t="s">
-        <v>209</v>
-      </c>
-      <c r="G101" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>206</v>
-      </c>
       <c r="B102" s="2" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="F102" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="G102" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>210</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>215</v>
+        <v>165</v>
       </c>
       <c r="F103" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="G103" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>211</v>
-      </c>
-      <c r="B104" s="2">
-        <v>47</v>
+        <v>226</v>
+      </c>
+      <c r="B104" t="s">
+        <v>218</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="D104" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F104" t="s">
+        <v>219</v>
+      </c>
+      <c r="G104" t="s">
         <v>220</v>
       </c>
-      <c r="F104" t="s">
-        <v>170</v>
-      </c>
-      <c r="G104" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>23</v>
+        <v>222</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="F105" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="G105" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>23</v>
+        <v>229</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>166</v>
+        <v>230</v>
       </c>
       <c r="F106" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="G106" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
+        <v>232</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B107" t="s">
-        <v>221</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="D107" s="1" t="s">
-        <v>138</v>
+        <v>234</v>
       </c>
       <c r="F107" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="G107" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="F108" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="G108" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>232</v>
+        <v>243</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>245</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="F109" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="G109" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>236</v>
+        <v>274</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>237</v>
+        <v>273</v>
       </c>
       <c r="F110" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="G110" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>242</v>
+        <v>137</v>
       </c>
       <c r="F111" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="G111" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C112" s="5" t="s">
-        <v>248</v>
+        <v>256</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>257</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>247</v>
+        <v>258</v>
+      </c>
+      <c r="F112" t="s">
+        <v>259</v>
       </c>
       <c r="G112" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F113" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="G113" t="s">
-        <v>117</v>
-      </c>
-      <c r="H113" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>138</v>
+        <v>268</v>
       </c>
       <c r="F114" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="G114" t="s">
-        <v>117</v>
-      </c>
-      <c r="H114" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="F115" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="G115" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>263</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F116" t="s">
-        <v>266</v>
-      </c>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G116" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>267</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F117" t="s">
-        <v>272</v>
-      </c>
-      <c r="G117" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>268</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="F118" t="s">
-        <v>275</v>
-      </c>
-      <c r="G118" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G119" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -3660,122 +3597,104 @@
     <hyperlink ref="D18" r:id="rId10" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL21A226MAQNNNE_22uF-226-20-25V_C45783.html/?href=jlc-SMT" xr:uid="{5CEE53D3-93BB-4898-A78E-B824EF492B70}"/>
     <hyperlink ref="D19" r:id="rId11" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL21A226MAQNNNE_22uF-226-20-25V_C45783.html/?href=jlc-SMT" xr:uid="{E6517C33-B5DC-4D0C-B8B8-4017294CB94B}"/>
     <hyperlink ref="D23" r:id="rId12" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_2-2nF-222-10-50V_C1604.html/?href=jlc-SMT" xr:uid="{F2E4924E-CBFF-4673-9E2F-E566A37DAE8B}"/>
-    <hyperlink ref="D26" r:id="rId13" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL21A106KAYNNNE_10uF-106-10-25V_C15850.html/?href=jlc-SMT" xr:uid="{E79B456F-DF3C-41CA-9EC5-3A1854B1DC54}"/>
-    <hyperlink ref="D28" r:id="rId14" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{DCCF458A-86AB-416E-9799-D1F946D39220}"/>
-    <hyperlink ref="D29" r:id="rId15" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{0AAB52A2-771F-4437-8EC6-5FD22F8F443A}"/>
-    <hyperlink ref="D30" r:id="rId16" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{387C0684-E2FA-4774-A36D-59AD787F5053}"/>
-    <hyperlink ref="D31" r:id="rId17" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_220pF-221-10-50V_C1530.html/?href=jlc-SMT" xr:uid="{59B80CC8-B5B1-44E2-AC3B-A8067C72598C}"/>
-    <hyperlink ref="D32" r:id="rId18" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_220pF-221-10-50V_C1530.html/?href=jlc-SMT" xr:uid="{02373A8F-5C04-4A7D-8922-00B5BA03E4E3}"/>
-    <hyperlink ref="D33" r:id="rId19" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_220pF-221-10-50V_C1530.html/?href=jlc-SMT" xr:uid="{052CCF65-8CBF-4B98-8A5F-D05A93AF4B62}"/>
-    <hyperlink ref="D34" r:id="rId20" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{0D80AB30-8E3C-4F13-8645-748AC65A1F08}"/>
-    <hyperlink ref="D35" r:id="rId21" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_12pF-120-5-50V_C1547.html/?href=jlc-SMT" xr:uid="{4669F01F-2F99-46FB-A6DA-4DCF89BBD5B8}"/>
-    <hyperlink ref="D36" r:id="rId22" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_12pF-120-5-50V_C1547.html/?href=jlc-SMT" xr:uid="{93D53298-3C35-4419-92C7-B1A8300DE74F}"/>
-    <hyperlink ref="D37" r:id="rId23" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_1nF-102-10-50V_C1523.html/?href=jlc-SMT" xr:uid="{CFC1F65C-5C26-4006-B7FA-F1EEDBF6C82E}"/>
-    <hyperlink ref="D38" r:id="rId24" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_12pF-120-5-50V_C1547.html/?href=jlc-SMT" xr:uid="{AF50C486-1405-4EC2-970E-49E66CC8DBC8}"/>
-    <hyperlink ref="D39" r:id="rId25" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05A105KA5NQNC_1uF-105-10-25V_C52923.html/?href=jlc-SMT" xr:uid="{80642DC3-9E7A-4E9C-ABFD-3E7C4668ED7F}"/>
-    <hyperlink ref="D41" r:id="rId26" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_12pF-120-5-50V_C1547.html/?href=jlc-SMT" xr:uid="{C7F02ACA-B30A-44A4-B42F-BCA2A7636ED8}"/>
-    <hyperlink ref="D40" r:id="rId27" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_1nF-102-10-50V_C1523.html/?href=jlc-SMT" xr:uid="{EEBC0943-269F-49BB-89AA-8935DDE4101F}"/>
-    <hyperlink ref="D42" r:id="rId28" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_2-2pF-2R2-0-25pF-50V_C1559.html/?href=jlc-SMT" xr:uid="{3821E901-7869-4BE2-ADF8-578AF88FC962}"/>
-    <hyperlink ref="D44" r:id="rId29" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_18pF-180-5-50V_C1549.html/?href=jlc-SMT" xr:uid="{F6F7D85F-95BA-4C7C-85A7-01FF8392CBA8}"/>
-    <hyperlink ref="D43" r:id="rId30" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_Murata-Electronics-GJM1555C1HR10WB01D_C161338.html/?href=jlc-SMT" xr:uid="{F7C41DA5-4377-4225-B264-397DCA9D8552}"/>
-    <hyperlink ref="D45" r:id="rId31" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05A105KA5NQNC_1uF-105-10-25V_C52923.html/?href=jlc-SMT" xr:uid="{3256BB23-11C3-4E1B-B78B-9A8A22DB09EE}"/>
-    <hyperlink ref="D46" r:id="rId32" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05A105KA5NQNC_1uF-105-10-25V_C52923.html/?href=jlc-SMT" xr:uid="{DA00E57D-90DB-4F73-A54D-0CE1604A2A2E}"/>
-    <hyperlink ref="D47" r:id="rId33" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_47pF-470-5-50V_C1567.html/?href=jlc-SMT" xr:uid="{ECE83CA2-5625-47EC-B304-EA0614492E3D}"/>
-    <hyperlink ref="D48" r:id="rId34" display="https://lcsc.com/product-detail/HF-Inductors_Sunlord-SDCL1005C10NJTDF_C27147.html/?href=jlc-SMT" xr:uid="{1DF8A7E8-E3AE-4027-BCD6-928334118A95}"/>
-    <hyperlink ref="D49" r:id="rId35" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_0603-Green-light_C72043.html/?href=jlc-SMT" xr:uid="{15B1E95E-7299-469E-A437-5D21FC77AEE4}"/>
-    <hyperlink ref="D50" r:id="rId36" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_Hubei-KENTO-Elec-KT-0603R_C2286.html/?href=jlc-SMT" xr:uid="{5D609E04-08AD-4DF0-A5EE-15804E3FBBEE}"/>
-    <hyperlink ref="D51" r:id="rId37" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_EKINGLUX-E6C0603SEAC1UDA_C375450.html/?href=jlc-SMT" xr:uid="{A56F321C-1FBF-4611-A52B-0EF9730F3235}"/>
-    <hyperlink ref="D52" r:id="rId38" xr:uid="{9DDC487F-977C-4719-856E-F6FEDA7DB520}"/>
-    <hyperlink ref="D58" r:id="rId39" xr:uid="{748B6806-9D55-4EDD-99F9-2256F6C1A641}"/>
-    <hyperlink ref="D59" r:id="rId40" xr:uid="{E3D1158C-5CA3-4570-9AA9-9023A6FEB1F9}"/>
-    <hyperlink ref="D62" r:id="rId41" xr:uid="{DBB0C382-8559-49E6-A39E-4DBF75A8205D}"/>
-    <hyperlink ref="D63" r:id="rId42" xr:uid="{DD35EFC3-AC2A-4C17-9910-90E1A8B3990B}"/>
-    <hyperlink ref="D60" r:id="rId43" xr:uid="{1EDA01AB-FBF7-43ED-9AFA-B8CDE41C9140}"/>
-    <hyperlink ref="D61" r:id="rId44" xr:uid="{435F8B9B-278E-4825-9298-39491C2B2727}"/>
-    <hyperlink ref="D64" r:id="rId45" display="https://lcsc.com/product-detail/HF-Inductors_Sunlord-SDCL1005C39NJTDF_C26443.html/?href=jlc-SMT" xr:uid="{E5820112-26BE-452E-AB6F-628C4B2EDF2D}"/>
-    <hyperlink ref="D65" r:id="rId46" display="https://lcsc.com/product-detail/HF-Inductors_Sunlord-SDCL1005C4N7STDF_C13595.html/?href=jlc-SMT" xr:uid="{C3472C7B-EDEC-4308-A347-2BACFDA1713B}"/>
-    <hyperlink ref="D66" r:id="rId47" display="https://lcsc.com/product-detail/HF-Inductors_Murata-Electronics_LQG15HS1N0S02D_Murata-Electronics-LQG15HS1N0S02D_C18222.html/?href=jlc-SMT" xr:uid="{F0E6495C-16BC-4D12-9204-E70542B847EE}"/>
-    <hyperlink ref="D67" r:id="rId48" display="https://lcsc.com/product-detail/HF-Inductors_Sunlord-SDCL1005C1N8STDF_C18304.html/?href=jlc-SMT" xr:uid="{E68421C6-F04F-461F-BE02-38DF45A8BB2B}"/>
-    <hyperlink ref="D68" r:id="rId49" display="https://lcsc.com/product-detail/HF-Inductors_Sunlord-SDCL1608C27NJTDF_C12100.html/?href=jlc-SMT" xr:uid="{6F315418-7930-4D8D-A7B3-EBBDDC046B20}"/>
-    <hyperlink ref="D69" r:id="rId50" display="https://lcsc.com/product-detail/MOSFET_Alpha-Omega-Semicon_AO3401A_Alpha-Omega-Semicon-AOS-AO3401A_C15127.html/?href=jlc-SMT" xr:uid="{9F0D050A-2B19-44D1-B82E-04CE79EF5C80}"/>
-    <hyperlink ref="D70" r:id="rId51" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1002TCE_C25744.html/?href=jlc-SMT" xr:uid="{91F0E965-6892-4E50-8199-95C1418A2DAB}"/>
-    <hyperlink ref="D71" r:id="rId52" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0805W8F470JT5E_C17714.html/?href=jlc-SMT" xr:uid="{2809CC4A-A974-4A27-89FA-B0A7D1FCB8EB}"/>
-    <hyperlink ref="D72" r:id="rId53" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1001TCE_C11702.html/?href=jlc-SMT" xr:uid="{8E00C76E-3DC1-469F-9613-3ED1BCC87777}"/>
-    <hyperlink ref="D73" r:id="rId54" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{D510D02A-3811-4E22-94CE-B5D8C855C848}"/>
-    <hyperlink ref="D74" r:id="rId55" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{A7D399F2-3328-42AB-8513-FED0DE5C8707}"/>
-    <hyperlink ref="D75" r:id="rId56" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{88D2E5AB-6BE4-4608-A52F-F64BEA2A68CA}"/>
-    <hyperlink ref="D76" r:id="rId57" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{78ED43F5-CF58-4AF0-A03C-257535C1C87B}"/>
-    <hyperlink ref="D77" r:id="rId58" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{9F872196-180E-4C80-A3A8-3DD8C066C2E9}"/>
-    <hyperlink ref="D78" r:id="rId59" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{C2AB56A9-61D5-48CD-AC90-276D7D7E04E0}"/>
-    <hyperlink ref="D79" r:id="rId60" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{846EE48B-F635-45DB-BE5B-3EBB79AF3569}"/>
-    <hyperlink ref="D80" r:id="rId61" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{D5B33C36-4098-4A28-A081-B0067B7EC0CF}"/>
-    <hyperlink ref="D81" r:id="rId62" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{CEAA0BB2-7128-4A7E-9A52-8ACB30DDECCB}"/>
-    <hyperlink ref="D82" r:id="rId63" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{2E06F9E5-8B55-4A32-8A59-F18CA60B1809}"/>
-    <hyperlink ref="D83" r:id="rId64" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{CC11A193-7BD5-4BB5-AE82-BBAD9456C83C}"/>
-    <hyperlink ref="D84" r:id="rId65" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{3B8C7B5F-A012-4569-AE67-EA7E941CFF67}"/>
-    <hyperlink ref="D85" r:id="rId66" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{7D5D5771-8841-4C25-BFF7-04808132ABE5}"/>
-    <hyperlink ref="D86" r:id="rId67" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{C3743F72-2A73-474E-982E-ED8B00C6F9BF}"/>
-    <hyperlink ref="D87" r:id="rId68" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{7CE96E79-266C-477D-8840-A0F40D0753CB}"/>
-    <hyperlink ref="D88" r:id="rId69" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{5C57A805-A27B-4FC1-B3C6-DDEFAD09235B}"/>
-    <hyperlink ref="D89" r:id="rId70" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{663CE9E2-0932-4E5B-9783-1E9D79730AFC}"/>
-    <hyperlink ref="D90" r:id="rId71" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{262D6504-07D8-4D44-A79F-413268ABEA34}"/>
-    <hyperlink ref="D91" r:id="rId72" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{059896D2-C86C-46E6-A918-BC8C85826163}"/>
-    <hyperlink ref="D92" r:id="rId73" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{A821F3D4-3D9A-45DB-9403-ED750A13F02E}"/>
-    <hyperlink ref="D93" r:id="rId74" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{1F26101D-B3E8-404C-A2A2-FE3DD0DDC5D6}"/>
-    <hyperlink ref="D94" r:id="rId75" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{796E71DE-2239-46EB-A514-CECD1DEFA63F}"/>
-    <hyperlink ref="D99" r:id="rId76" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1001TCE_C11702.html/?href=jlc-SMT" xr:uid="{051F061C-DE3E-42C5-9FF0-E184567786DE}"/>
-    <hyperlink ref="D95" r:id="rId77" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF4701TCE_C25900.html/?href=jlc-SMT" xr:uid="{5C6FBD3D-563C-45DC-88B1-D7B67F55B108}"/>
-    <hyperlink ref="D96:D98" r:id="rId78" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF4701TCE_C25900.html/?href=jlc-SMT" xr:uid="{10440215-2E29-42A7-8BD1-D1FEC63A50B3}"/>
-    <hyperlink ref="D100" r:id="rId79" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF4701TCE_C25900.html/?href=jlc-SMT" xr:uid="{64841EC7-AA32-47E2-8504-8F361625326D}"/>
-    <hyperlink ref="D101:D102" r:id="rId80" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF4701TCE_C25900.html/?href=jlc-SMT" xr:uid="{DF40ED35-8CCC-4C46-BB7E-B86503718063}"/>
-    <hyperlink ref="D103" r:id="rId81" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF5602TCE_C25796.html/?href=jlc-SMT" xr:uid="{66A35609-AD82-4995-BA37-2795B95D88B2}"/>
-    <hyperlink ref="D105" r:id="rId82" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF3901TCE_C51721.html/?href=jlc-SMT" xr:uid="{E511C1B9-5CE6-43D2-88A7-EE2D8FF5A38C}"/>
-    <hyperlink ref="D106" r:id="rId83" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1002TCE_C25744.html/?href=jlc-SMT" xr:uid="{C41E5EEE-1C99-4F38-BF8B-F8E601EA695F}"/>
-    <hyperlink ref="D104" r:id="rId84" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF470JTCE_C25118.html/?href=jlc-SMT" xr:uid="{8675A7AF-01D2-4808-AE85-57282F9806F1}"/>
-    <hyperlink ref="D107" r:id="rId85" xr:uid="{A928FBB0-FBAF-4759-931A-556AD9F4359C}"/>
-    <hyperlink ref="D108" r:id="rId86" display="https://lcsc.com/product-detail/ST-Microelectronics_STMicroelectronics_STM32F407VGT6_STM32F407VGT6_C12345.html/?href=jlc-SMT" xr:uid="{FF079FAB-EED7-421B-8DF7-058F8CD0A515}"/>
-    <hyperlink ref="D109" r:id="rId87" display="https://lcsc.com/product-detail/Low-Dropout-Regulators-LDO_AMS_AMS1117-3-3_AMS1117-3-3_C6186.html/?href=jlc-SMT" xr:uid="{C88640B3-D15B-48A4-89D7-3412C4456249}"/>
-    <hyperlink ref="D110" r:id="rId88" display="https://lcsc.com/product-detail/Low-Dropout-Regulators-LDO_AMS_AMS1117-5-0_AMS1117-5-0_C6187.html/?href=jlc-SMT" xr:uid="{4D468AE9-B2FF-4CF0-9C6B-626AADE8D825}"/>
-    <hyperlink ref="D111" r:id="rId89" display="https://lcsc.com/product-detail/Attitude-Sensors_TDK-InvenSense_MPU-6050_TDK-InvenSense-MPU-6050_C24112.html/?href=jlc-SMT" xr:uid="{29BA538D-A230-4C58-A40B-BEEFB6CF5182}"/>
-    <hyperlink ref="D112" r:id="rId90" display="https://lcsc.com/product-detail/FLASH_Winbond-Elec-W25N01GVZEIG_C88868.html/?href=jlc-SMT" xr:uid="{B5AD234F-BE13-44CB-A323-79CCC3A7F316}"/>
-    <hyperlink ref="H113" r:id="rId91" display="https://lcsc.com/product-detail/Sensors_FREESCALE_MPL3115A2R1_MPL3115A2R1_C54429.html/?href=jlc-SMT" xr:uid="{9410E4B7-FCD8-46D2-8753-EBD835E7DE9C}"/>
-    <hyperlink ref="D113" r:id="rId92" xr:uid="{0A004393-A8E8-487C-B8B0-84A159554335}"/>
-    <hyperlink ref="H114" r:id="rId93" display="https://lcsc.com/product-detail/RF-Chips_Texas-Instruments_CC2500RGPR_Texas-Instruments-TI-CC2500RGPR_C57494.html/?href=jlc-SMT" xr:uid="{4D765861-9E01-49A5-9428-ACA729A00DC6}"/>
-    <hyperlink ref="D114" r:id="rId94" xr:uid="{539A0D58-D948-4AD1-B1FD-B0A6F8687637}"/>
-    <hyperlink ref="D115" r:id="rId95" display="https://lcsc.com/product-detail/RF-Transceiver-ICs_Texas-Instruments_CC2592RGVR_Texas-Instruments-TI-CC2592RGVR_C53274.html/?href=jlc-SMT" xr:uid="{67ABE811-0156-4B04-A7B9-CB402BA96858}"/>
-    <hyperlink ref="D116" r:id="rId96" xr:uid="{F43067F2-49FF-4F7C-94A2-CAA12E64CF29}"/>
-    <hyperlink ref="D117" r:id="rId97" display="https://lcsc.com/product-detail/SMD-Crystal-Resonators_Yangxing-Tech-X322516MLB4SI_C13738.html/?href=jlc-SMT" xr:uid="{AFCEF283-9E23-4C17-AD98-C2B16E2C3008}"/>
-    <hyperlink ref="D118" r:id="rId98" display="https://lcsc.com/product-detail/SMD-Crystal-Resonators_Yangxing-Tech-X322526MEB4SC_C23425.html/?href=jlc-SMT" xr:uid="{5C8D8D15-8C9E-4CAB-B7CC-92CEABBE5CD7}"/>
-    <hyperlink ref="D3" r:id="rId99" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{8833A834-89E4-4FC8-AE18-1D501717B49D}"/>
-    <hyperlink ref="D20" r:id="rId100" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{D212AD37-2141-4E02-9CD1-6FE05EE9DA92}"/>
-    <hyperlink ref="D21" r:id="rId101" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{FA7CC880-D27D-4023-8136-306901D2D3C3}"/>
-    <hyperlink ref="D22" r:id="rId102" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{59191488-15A4-443C-AACE-74ACC99423C2}"/>
-    <hyperlink ref="D24" r:id="rId103" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{05118BBC-FE14-4394-BC96-EA2BCCE3E953}"/>
-    <hyperlink ref="D4:D9" r:id="rId104" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{762A4A00-5288-4F1A-AD22-EC5BDA7C3ACA}"/>
-    <hyperlink ref="D25" r:id="rId105" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{2AD975E5-144E-4FD6-8FAC-52A21AE3CBE6}"/>
-    <hyperlink ref="D27" r:id="rId106" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{43AC85BC-B4E7-4E21-83AC-0B5DC6AFE853}"/>
+    <hyperlink ref="D25" r:id="rId13" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL21A106KAYNNNE_10uF-106-10-25V_C15850.html/?href=jlc-SMT" xr:uid="{E79B456F-DF3C-41CA-9EC5-3A1854B1DC54}"/>
+    <hyperlink ref="D27" r:id="rId14" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{DCCF458A-86AB-416E-9799-D1F946D39220}"/>
+    <hyperlink ref="D28" r:id="rId15" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{0AAB52A2-771F-4437-8EC6-5FD22F8F443A}"/>
+    <hyperlink ref="D29" r:id="rId16" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{387C0684-E2FA-4774-A36D-59AD787F5053}"/>
+    <hyperlink ref="D30" r:id="rId17" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_220pF-221-10-50V_C1530.html/?href=jlc-SMT" xr:uid="{59B80CC8-B5B1-44E2-AC3B-A8067C72598C}"/>
+    <hyperlink ref="D31" r:id="rId18" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_220pF-221-10-50V_C1530.html/?href=jlc-SMT" xr:uid="{02373A8F-5C04-4A7D-8922-00B5BA03E4E3}"/>
+    <hyperlink ref="D32" r:id="rId19" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_220pF-221-10-50V_C1530.html/?href=jlc-SMT" xr:uid="{052CCF65-8CBF-4B98-8A5F-D05A93AF4B62}"/>
+    <hyperlink ref="D33" r:id="rId20" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{0D80AB30-8E3C-4F13-8645-748AC65A1F08}"/>
+    <hyperlink ref="D34" r:id="rId21" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_12pF-120-5-50V_C1547.html/?href=jlc-SMT" xr:uid="{4669F01F-2F99-46FB-A6DA-4DCF89BBD5B8}"/>
+    <hyperlink ref="D35" r:id="rId22" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_12pF-120-5-50V_C1547.html/?href=jlc-SMT" xr:uid="{93D53298-3C35-4419-92C7-B1A8300DE74F}"/>
+    <hyperlink ref="D36" r:id="rId23" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_1nF-102-10-50V_C1523.html/?href=jlc-SMT" xr:uid="{CFC1F65C-5C26-4006-B7FA-F1EEDBF6C82E}"/>
+    <hyperlink ref="D37" r:id="rId24" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_12pF-120-5-50V_C1547.html/?href=jlc-SMT" xr:uid="{AF50C486-1405-4EC2-970E-49E66CC8DBC8}"/>
+    <hyperlink ref="D38" r:id="rId25" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05A105KA5NQNC_1uF-105-10-25V_C52923.html/?href=jlc-SMT" xr:uid="{80642DC3-9E7A-4E9C-ABFD-3E7C4668ED7F}"/>
+    <hyperlink ref="D40" r:id="rId26" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_12pF-120-5-50V_C1547.html/?href=jlc-SMT" xr:uid="{C7F02ACA-B30A-44A4-B42F-BCA2A7636ED8}"/>
+    <hyperlink ref="D39" r:id="rId27" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_1nF-102-10-50V_C1523.html/?href=jlc-SMT" xr:uid="{EEBC0943-269F-49BB-89AA-8935DDE4101F}"/>
+    <hyperlink ref="D41" r:id="rId28" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_2-2pF-2R2-0-25pF-50V_C1559.html/?href=jlc-SMT" xr:uid="{3821E901-7869-4BE2-ADF8-578AF88FC962}"/>
+    <hyperlink ref="D43" r:id="rId29" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_18pF-180-5-50V_C1549.html/?href=jlc-SMT" xr:uid="{F6F7D85F-95BA-4C7C-85A7-01FF8392CBA8}"/>
+    <hyperlink ref="D42" r:id="rId30" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_Murata-Electronics-GJM1555C1HR10WB01D_C161338.html/?href=jlc-SMT" xr:uid="{F7C41DA5-4377-4225-B264-397DCA9D8552}"/>
+    <hyperlink ref="D44" r:id="rId31" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05A105KA5NQNC_1uF-105-10-25V_C52923.html/?href=jlc-SMT" xr:uid="{3256BB23-11C3-4E1B-B78B-9A8A22DB09EE}"/>
+    <hyperlink ref="D45" r:id="rId32" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05A105KA5NQNC_1uF-105-10-25V_C52923.html/?href=jlc-SMT" xr:uid="{DA00E57D-90DB-4F73-A54D-0CE1604A2A2E}"/>
+    <hyperlink ref="D46" r:id="rId33" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_47pF-470-5-50V_C1567.html/?href=jlc-SMT" xr:uid="{ECE83CA2-5625-47EC-B304-EA0614492E3D}"/>
+    <hyperlink ref="D47" r:id="rId34" display="https://lcsc.com/product-detail/HF-Inductors_Sunlord-SDCL1005C10NJTDF_C27147.html/?href=jlc-SMT" xr:uid="{1DF8A7E8-E3AE-4027-BCD6-928334118A95}"/>
+    <hyperlink ref="D48" r:id="rId35" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_0603-Green-light_C72043.html/?href=jlc-SMT" xr:uid="{15B1E95E-7299-469E-A437-5D21FC77AEE4}"/>
+    <hyperlink ref="D49" r:id="rId36" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_Hubei-KENTO-Elec-KT-0603R_C2286.html/?href=jlc-SMT" xr:uid="{5D609E04-08AD-4DF0-A5EE-15804E3FBBEE}"/>
+    <hyperlink ref="D50" r:id="rId37" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_EKINGLUX-E6C0603SEAC1UDA_C375450.html/?href=jlc-SMT" xr:uid="{A56F321C-1FBF-4611-A52B-0EF9730F3235}"/>
+    <hyperlink ref="D51" r:id="rId38" xr:uid="{9DDC487F-977C-4719-856E-F6FEDA7DB520}"/>
+    <hyperlink ref="D57" r:id="rId39" xr:uid="{748B6806-9D55-4EDD-99F9-2256F6C1A641}"/>
+    <hyperlink ref="D58" r:id="rId40" xr:uid="{E3D1158C-5CA3-4570-9AA9-9023A6FEB1F9}"/>
+    <hyperlink ref="D61" r:id="rId41" xr:uid="{DBB0C382-8559-49E6-A39E-4DBF75A8205D}"/>
+    <hyperlink ref="D62" r:id="rId42" xr:uid="{DD35EFC3-AC2A-4C17-9910-90E1A8B3990B}"/>
+    <hyperlink ref="D59" r:id="rId43" xr:uid="{1EDA01AB-FBF7-43ED-9AFA-B8CDE41C9140}"/>
+    <hyperlink ref="D60" r:id="rId44" xr:uid="{435F8B9B-278E-4825-9298-39491C2B2727}"/>
+    <hyperlink ref="D63" r:id="rId45" display="https://lcsc.com/product-detail/HF-Inductors_Sunlord-SDCL1005C39NJTDF_C26443.html/?href=jlc-SMT" xr:uid="{E5820112-26BE-452E-AB6F-628C4B2EDF2D}"/>
+    <hyperlink ref="D64" r:id="rId46" display="https://lcsc.com/product-detail/HF-Inductors_Sunlord-SDCL1005C4N7STDF_C13595.html/?href=jlc-SMT" xr:uid="{C3472C7B-EDEC-4308-A347-2BACFDA1713B}"/>
+    <hyperlink ref="D65" r:id="rId47" display="https://lcsc.com/product-detail/HF-Inductors_Murata-Electronics_LQG15HS1N0S02D_Murata-Electronics-LQG15HS1N0S02D_C18222.html/?href=jlc-SMT" xr:uid="{F0E6495C-16BC-4D12-9204-E70542B847EE}"/>
+    <hyperlink ref="D66" r:id="rId48" display="https://lcsc.com/product-detail/HF-Inductors_Sunlord-SDCL1005C1N8STDF_C18304.html/?href=jlc-SMT" xr:uid="{E68421C6-F04F-461F-BE02-38DF45A8BB2B}"/>
+    <hyperlink ref="D67" r:id="rId49" display="https://lcsc.com/product-detail/HF-Inductors_Sunlord-SDCL1608C27NJTDF_C12100.html/?href=jlc-SMT" xr:uid="{6F315418-7930-4D8D-A7B3-EBBDDC046B20}"/>
+    <hyperlink ref="D68" r:id="rId50" display="https://lcsc.com/product-detail/MOSFET_Alpha-Omega-Semicon_AO3401A_Alpha-Omega-Semicon-AOS-AO3401A_C15127.html/?href=jlc-SMT" xr:uid="{9F0D050A-2B19-44D1-B82E-04CE79EF5C80}"/>
+    <hyperlink ref="D69" r:id="rId51" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1002TCE_C25744.html/?href=jlc-SMT" xr:uid="{91F0E965-6892-4E50-8199-95C1418A2DAB}"/>
+    <hyperlink ref="D70" r:id="rId52" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0805W8F470JT5E_C17714.html/?href=jlc-SMT" xr:uid="{2809CC4A-A974-4A27-89FA-B0A7D1FCB8EB}"/>
+    <hyperlink ref="D71" r:id="rId53" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1001TCE_C11702.html/?href=jlc-SMT" xr:uid="{8E00C76E-3DC1-469F-9613-3ED1BCC87777}"/>
+    <hyperlink ref="D72" r:id="rId54" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{D510D02A-3811-4E22-94CE-B5D8C855C848}"/>
+    <hyperlink ref="D73" r:id="rId55" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{A7D399F2-3328-42AB-8513-FED0DE5C8707}"/>
+    <hyperlink ref="D74" r:id="rId56" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{88D2E5AB-6BE4-4608-A52F-F64BEA2A68CA}"/>
+    <hyperlink ref="D75" r:id="rId57" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{78ED43F5-CF58-4AF0-A03C-257535C1C87B}"/>
+    <hyperlink ref="D76" r:id="rId58" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{9F872196-180E-4C80-A3A8-3DD8C066C2E9}"/>
+    <hyperlink ref="D77" r:id="rId59" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{C2AB56A9-61D5-48CD-AC90-276D7D7E04E0}"/>
+    <hyperlink ref="D78" r:id="rId60" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{846EE48B-F635-45DB-BE5B-3EBB79AF3569}"/>
+    <hyperlink ref="D79" r:id="rId61" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{D5B33C36-4098-4A28-A081-B0067B7EC0CF}"/>
+    <hyperlink ref="D80" r:id="rId62" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{CEAA0BB2-7128-4A7E-9A52-8ACB30DDECCB}"/>
+    <hyperlink ref="D81" r:id="rId63" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{2E06F9E5-8B55-4A32-8A59-F18CA60B1809}"/>
+    <hyperlink ref="D82" r:id="rId64" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{CC11A193-7BD5-4BB5-AE82-BBAD9456C83C}"/>
+    <hyperlink ref="D83" r:id="rId65" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{3B8C7B5F-A012-4569-AE67-EA7E941CFF67}"/>
+    <hyperlink ref="D84" r:id="rId66" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{7D5D5771-8841-4C25-BFF7-04808132ABE5}"/>
+    <hyperlink ref="D85" r:id="rId67" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{C3743F72-2A73-474E-982E-ED8B00C6F9BF}"/>
+    <hyperlink ref="D86" r:id="rId68" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{7CE96E79-266C-477D-8840-A0F40D0753CB}"/>
+    <hyperlink ref="D87" r:id="rId69" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{5C57A805-A27B-4FC1-B3C6-DDEFAD09235B}"/>
+    <hyperlink ref="D88" r:id="rId70" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{663CE9E2-0932-4E5B-9783-1E9D79730AFC}"/>
+    <hyperlink ref="D89" r:id="rId71" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{262D6504-07D8-4D44-A79F-413268ABEA34}"/>
+    <hyperlink ref="D90" r:id="rId72" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{059896D2-C86C-46E6-A918-BC8C85826163}"/>
+    <hyperlink ref="D91" r:id="rId73" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{A821F3D4-3D9A-45DB-9403-ED750A13F02E}"/>
+    <hyperlink ref="D96" r:id="rId74" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1001TCE_C11702.html/?href=jlc-SMT" xr:uid="{051F061C-DE3E-42C5-9FF0-E184567786DE}"/>
+    <hyperlink ref="D92" r:id="rId75" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF4701TCE_C25900.html/?href=jlc-SMT" xr:uid="{5C6FBD3D-563C-45DC-88B1-D7B67F55B108}"/>
+    <hyperlink ref="D93:D95" r:id="rId76" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF4701TCE_C25900.html/?href=jlc-SMT" xr:uid="{10440215-2E29-42A7-8BD1-D1FEC63A50B3}"/>
+    <hyperlink ref="D97" r:id="rId77" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF4701TCE_C25900.html/?href=jlc-SMT" xr:uid="{64841EC7-AA32-47E2-8504-8F361625326D}"/>
+    <hyperlink ref="D98:D99" r:id="rId78" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF4701TCE_C25900.html/?href=jlc-SMT" xr:uid="{DF40ED35-8CCC-4C46-BB7E-B86503718063}"/>
+    <hyperlink ref="D100" r:id="rId79" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF5602TCE_C25796.html/?href=jlc-SMT" xr:uid="{66A35609-AD82-4995-BA37-2795B95D88B2}"/>
+    <hyperlink ref="D102" r:id="rId80" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF3901TCE_C51721.html/?href=jlc-SMT" xr:uid="{E511C1B9-5CE6-43D2-88A7-EE2D8FF5A38C}"/>
+    <hyperlink ref="D103" r:id="rId81" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1002TCE_C25744.html/?href=jlc-SMT" xr:uid="{C41E5EEE-1C99-4F38-BF8B-F8E601EA695F}"/>
+    <hyperlink ref="D101" r:id="rId82" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF470JTCE_C25118.html/?href=jlc-SMT" xr:uid="{8675A7AF-01D2-4808-AE85-57282F9806F1}"/>
+    <hyperlink ref="D104" r:id="rId83" xr:uid="{A928FBB0-FBAF-4759-931A-556AD9F4359C}"/>
+    <hyperlink ref="D105" r:id="rId84" display="https://lcsc.com/product-detail/ST-Microelectronics_STMicroelectronics_STM32F407VGT6_STM32F407VGT6_C12345.html/?href=jlc-SMT" xr:uid="{FF079FAB-EED7-421B-8DF7-058F8CD0A515}"/>
+    <hyperlink ref="D106" r:id="rId85" display="https://lcsc.com/product-detail/Low-Dropout-Regulators-LDO_AMS_AMS1117-3-3_AMS1117-3-3_C6186.html/?href=jlc-SMT" xr:uid="{C88640B3-D15B-48A4-89D7-3412C4456249}"/>
+    <hyperlink ref="D107" r:id="rId86" display="https://lcsc.com/product-detail/Low-Dropout-Regulators-LDO_AMS_AMS1117-5-0_AMS1117-5-0_C6187.html/?href=jlc-SMT" xr:uid="{4D468AE9-B2FF-4CF0-9C6B-626AADE8D825}"/>
+    <hyperlink ref="D108" r:id="rId87" display="https://lcsc.com/product-detail/Attitude-Sensors_TDK-InvenSense_MPU-6050_TDK-InvenSense-MPU-6050_C24112.html/?href=jlc-SMT" xr:uid="{29BA538D-A230-4C58-A40B-BEEFB6CF5182}"/>
+    <hyperlink ref="D109" r:id="rId88" display="https://lcsc.com/product-detail/FLASH_Winbond-Elec-W25N01GVZEIG_C88868.html/?href=jlc-SMT" xr:uid="{B5AD234F-BE13-44CB-A323-79CCC3A7F316}"/>
+    <hyperlink ref="H110" r:id="rId89" display="https://lcsc.com/product-detail/Sensors_FREESCALE_MPL3115A2R1_MPL3115A2R1_C54429.html/?href=jlc-SMT" xr:uid="{9410E4B7-FCD8-46D2-8753-EBD835E7DE9C}"/>
+    <hyperlink ref="H111" r:id="rId90" display="https://lcsc.com/product-detail/RF-Chips_Texas-Instruments_CC2500RGPR_Texas-Instruments-TI-CC2500RGPR_C57494.html/?href=jlc-SMT" xr:uid="{4D765861-9E01-49A5-9428-ACA729A00DC6}"/>
+    <hyperlink ref="D111" r:id="rId91" xr:uid="{539A0D58-D948-4AD1-B1FD-B0A6F8687637}"/>
+    <hyperlink ref="D112" r:id="rId92" display="https://lcsc.com/product-detail/RF-Transceiver-ICs_Texas-Instruments_CC2592RGVR_Texas-Instruments-TI-CC2592RGVR_C53274.html/?href=jlc-SMT" xr:uid="{67ABE811-0156-4B04-A7B9-CB402BA96858}"/>
+    <hyperlink ref="D113" r:id="rId93" xr:uid="{F43067F2-49FF-4F7C-94A2-CAA12E64CF29}"/>
+    <hyperlink ref="D114" r:id="rId94" display="https://lcsc.com/product-detail/SMD-Crystal-Resonators_Yangxing-Tech-X322516MLB4SI_C13738.html/?href=jlc-SMT" xr:uid="{AFCEF283-9E23-4C17-AD98-C2B16E2C3008}"/>
+    <hyperlink ref="D115" r:id="rId95" display="https://lcsc.com/product-detail/SMD-Crystal-Resonators_Yangxing-Tech-X322526MEB4SC_C23425.html/?href=jlc-SMT" xr:uid="{5C8D8D15-8C9E-4CAB-B7CC-92CEABBE5CD7}"/>
+    <hyperlink ref="D3" r:id="rId96" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{8833A834-89E4-4FC8-AE18-1D501717B49D}"/>
+    <hyperlink ref="D20" r:id="rId97" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{D212AD37-2141-4E02-9CD1-6FE05EE9DA92}"/>
+    <hyperlink ref="D21" r:id="rId98" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{FA7CC880-D27D-4023-8136-306901D2D3C3}"/>
+    <hyperlink ref="D22" r:id="rId99" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{59191488-15A4-443C-AACE-74ACC99423C2}"/>
+    <hyperlink ref="D24" r:id="rId100" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{05118BBC-FE14-4394-BC96-EA2BCCE3E953}"/>
+    <hyperlink ref="D4:D9" r:id="rId101" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{762A4A00-5288-4F1A-AD22-EC5BDA7C3ACA}"/>
+    <hyperlink ref="D26" r:id="rId102" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{43AC85BC-B4E7-4E21-83AC-0B5DC6AFE853}"/>
+    <hyperlink ref="D110" r:id="rId103" display="https://lcsc.com/product-detail/Pressure-Sensors_STMicroelectronics-LPS25HBTR_C87898.html/?href=jlc-SMT" xr:uid="{69A1E959-76C3-48CC-B7FE-A84746EADDB5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId107"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId104"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006A026355BAD2274782A07C8F49662C6C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb6eea23527ae3a2f4369f132760501b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="21dd6821-497d-487e-9974-da04441ecaef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3478fcf4c6a9925f36af177c8bf0c567" ns3:_="">
     <xsd:import namespace="21dd6821-497d-487e-9974-da04441ecaef"/>
@@ -3907,31 +3826,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AD7D0BB-8B92-4CB9-B3D0-89246867E7A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="21dd6821-497d-487e-9974-da04441ecaef"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{945E74FF-CF67-48D5-9BFC-8913C1D8D26C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4231A569-AFE9-4217-B34A-0C0809A85203}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3947,4 +3857,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{945E74FF-CF67-48D5-9BFC-8913C1D8D26C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AD7D0BB-8B92-4CB9-B3D0-89246867E7A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="21dd6821-497d-487e-9974-da04441ecaef"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>